<commit_message>
changed counts to 0
</commit_message>
<xml_diff>
--- a/Joe1.xlsx
+++ b/Joe1.xlsx
@@ -367,7 +367,7 @@
     <t xml:space="preserve">1.09 (range: 0.00 to 88.75)</t>
   </si>
   <si>
-    <t xml:space="preserve">8,828 (range: 11 to 169,257)</t>
+    <t xml:space="preserve">7,170 (range: 0 to 169,257)</t>
   </si>
   <si>
     <t xml:space="preserve">389 (85%)</t>
@@ -1452,48 +1452,40 @@
     </row>
     <row r="80" ht="NA" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B80" s="9" t="n">
-        <v>86</v>
+        <v>73</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="81" ht="NA" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" ht="NA" customHeight="1">
-      <c r="A82" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="83" ht="NA" customHeight="1">
-      <c r="A83" s="5" t="s">
+      <c r="A82" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="B82" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="6" t="s">
+    <row r="83">
+      <c r="A83" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B84" s="6" t="s">
+      <c r="B83" s="6" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A83:B83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>